<commit_message>
Final touch for GUI
</commit_message>
<xml_diff>
--- a/DATA/log/logbook_2025_11.xlsx
+++ b/DATA/log/logbook_2025_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1683,6 +1683,57 @@
         <v>1.78</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-11-26 00:44:49</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>A873-150925-CHK-Y06</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>993</v>
+      </c>
+      <c r="E25" t="n">
+        <v>993</v>
+      </c>
+      <c r="F25" t="n">
+        <v>951</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>25</v>
+      </c>
+      <c r="I25" t="n">
+        <v>17</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>813</v>
+      </c>
+      <c r="L25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>42</v>
+      </c>
+      <c r="N25" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1.96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update input source option
</commit_message>
<xml_diff>
--- a/DATA/log/logbook_2025_11.xlsx
+++ b/DATA/log/logbook_2025_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1734,6 +1734,57 @@
         <v>1.96</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-11-29 16:40:54</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>A873-150925-CHK-Y06</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>891</v>
+      </c>
+      <c r="E26" t="n">
+        <v>891</v>
+      </c>
+      <c r="F26" t="n">
+        <v>881</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>9</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>631</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>10</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O26" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing the status column of the GUI
</commit_message>
<xml_diff>
--- a/DATA/log/logbook_2025_11.xlsx
+++ b/DATA/log/logbook_2025_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2703,6 +2703,159 @@
         <v>3.17</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025-11-30 00:34:56</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>A605-010525-CHK-Y12</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>3988</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3988</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3890</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" t="n">
+        <v>93</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>4</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1963</v>
+      </c>
+      <c r="L45" t="b">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>97</v>
+      </c>
+      <c r="N45" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="O45" t="n">
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025-11-30 00:49:07</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>A873-150925-CHK-Y06</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>891</v>
+      </c>
+      <c r="E46" t="n">
+        <v>891</v>
+      </c>
+      <c r="F46" t="n">
+        <v>881</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>9</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" t="n">
+        <v>631</v>
+      </c>
+      <c r="L46" t="b">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>10</v>
+      </c>
+      <c r="N46" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O46" t="n">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2025-11-30 00:49:24</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>A605-010525-CHK-Y12</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>3988</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3988</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3890</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" t="n">
+        <v>93</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>4</v>
+      </c>
+      <c r="K47" t="n">
+        <v>1963</v>
+      </c>
+      <c r="L47" t="b">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>97</v>
+      </c>
+      <c r="N47" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="O47" t="n">
+        <v>11.21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>